<commit_message>
day-08 completed. pandas major functions and tricks
</commit_message>
<xml_diff>
--- a/day_06/data.xlsx
+++ b/day_06/data.xlsx
@@ -111,7 +111,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,7 +428,7 @@
     <col min="3" max="3" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="4">
         <v>5.8</v>
       </c>
@@ -450,7 +450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="4">
         <v>6.2</v>
       </c>
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="4">
         <v>5.9</v>
       </c>
@@ -472,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="4">
         <v>5.9</v>
       </c>
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="4">
         <v>5.9</v>
       </c>
@@ -494,7 +494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="4">
         <v>5.3</v>
       </c>
@@ -505,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="4">
         <v>5.6</v>
       </c>
@@ -516,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="4">
         <v>5.9</v>
       </c>
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" hidden="1">
       <c r="A10" s="4">
         <v>5.1</v>
       </c>
@@ -538,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="4">
         <v>5.4</v>
       </c>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" hidden="1">
       <c r="A12" s="4">
         <v>5.11</v>
       </c>
@@ -560,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="4">
         <v>5.7</v>
       </c>
@@ -571,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="1">
         <v>6.1</v>
       </c>
@@ -582,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="4">
         <v>5.7</v>
       </c>
@@ -593,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="4">
         <v>5.8</v>
       </c>
@@ -604,7 +604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="5">
         <v>5</v>
       </c>
@@ -615,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="4">
         <v>5.7</v>
       </c>
@@ -626,7 +626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="4">
         <v>5.9</v>
       </c>
@@ -637,7 +637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="4">
         <v>5.8</v>
       </c>
@@ -648,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="4">
         <v>5.5</v>
       </c>
@@ -659,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="5">
         <v>6</v>
       </c>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="4">
         <v>5.6</v>
       </c>
@@ -681,7 +681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="4">
         <v>5.8</v>
       </c>
@@ -692,7 +692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="4">
         <v>5.7</v>
       </c>
@@ -703,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="4">
         <v>5.3</v>
       </c>
@@ -714,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -725,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="5">
         <v>5</v>
       </c>
@@ -736,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" hidden="1">
       <c r="A29" s="4">
         <v>5.11</v>
       </c>
@@ -747,7 +747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="1">
         <v>5.8</v>
       </c>
@@ -758,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="4">
         <v>5.4</v>
       </c>
@@ -769,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25" hidden="1">
       <c r="A32" s="4">
         <v>5.1</v>
       </c>
@@ -780,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="4">
         <v>5.9</v>
       </c>
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="4">
         <v>5.9</v>
       </c>
@@ -802,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" hidden="1">
       <c r="A35" s="4">
         <v>5.1</v>
       </c>
@@ -813,7 +813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="5">
         <v>6</v>
       </c>
@@ -824,7 +824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="5">
         <v>5</v>
       </c>
@@ -835,7 +835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="4">
         <v>5.7</v>
       </c>
@@ -846,7 +846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="4">
         <v>5.6</v>
       </c>
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" hidden="1">
       <c r="A40" s="4">
         <v>5.1</v>
       </c>
@@ -868,7 +868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" hidden="1">
       <c r="A41" s="1">
         <v>5.11</v>
       </c>
@@ -879,7 +879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="5">
         <v>5</v>
       </c>
@@ -890,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="1">
         <v>5.6</v>
       </c>
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="4">
         <v>5.6</v>
       </c>
@@ -912,7 +912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="5">
         <v>59</v>
       </c>
@@ -923,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="4">
         <v>5.2</v>
       </c>
@@ -934,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="5">
         <v>167</v>
       </c>
@@ -945,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="4">
         <v>5.8</v>
       </c>
@@ -956,7 +956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="4">
         <v>5.9</v>
       </c>
@@ -967,7 +967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="4">
         <v>5.6</v>
       </c>
@@ -978,7 +978,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="4">
         <v>5.4</v>
       </c>
@@ -989,7 +989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="1">
         <v>5.7</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="1">
         <v>5.9</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="4">
         <v>5.7</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="4">
         <v>5.2</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="1">
         <v>5.8</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="4">
         <v>5.8</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="1">
         <v>5.3</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" hidden="1">
       <c r="A59" s="4">
         <v>5.1</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="1">
         <v>5.9</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="4">
         <v>5.2</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="5">
         <v>6</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="4">
         <v>5.5</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25" hidden="1">
       <c r="A64" s="4">
         <v>5.11</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="4">
         <v>5.2</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
       <c r="A66" s="1">
         <v>5.4</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25" hidden="1">
       <c r="A71" s="4">
         <v>5.1</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25" hidden="1">
       <c r="A75" s="1">
         <v>5.11</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25" hidden="1">
       <c r="A80" s="1">
         <v>5.11</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25" hidden="1">
       <c r="A88" s="4">
         <v>5.1</v>
       </c>

</xml_diff>